<commit_message>
feat: menu auto fit to screen
</commit_message>
<xml_diff>
--- a/public/Menu_FoodCourt.xlsx
+++ b/public/Menu_FoodCourt.xlsx
@@ -6,9 +6,9 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
@@ -42,97 +42,99 @@
     <t xml:space="preserve">Cuisine du monde </t>
   </si>
   <si>
+    <t xml:space="preserve">Curry panang </t>
+  </si>
+  <si>
+    <t>16.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fourchette Verte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lasagne au boeuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouquet de salades</t>
+  </si>
+  <si>
+    <t>10.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.40 prix apprenti·e·s</t>
+  </si>
+  <si>
+    <t>Lundi</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Cheeseburger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pommes frites</t>
+  </si>
+  <si>
+    <t>19.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baguette merguez</t>
+  </si>
+  <si>
+    <t>13.-</t>
+  </si>
+  <si>
+    <t>Mardi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bo Bun au boeuf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saladine de roquette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panini mozzarella et pesto rosso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salade mêlée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken Lousiana burger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrimps Po' Boy</t>
+  </si>
+  <si>
+    <t>Mercredi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couscous à l'agneau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tajine de légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schnitzel de poulet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pommes duchesse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot fondue</t>
+  </si>
+  <si>
+    <t>Jeudi</t>
+  </si>
+  <si>
+    <t>Gyros</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orzotto à la courge et Grana Panado</t>
   </si>
   <si>
-    <t>16.-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fourchette Verte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lasagne
-au boeuf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bouquet de salades</t>
-  </si>
-  <si>
-    <t>10.-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.40 prix apprenti·e·s</t>
-  </si>
-  <si>
-    <t>Lundi</t>
-  </si>
-  <si>
-    <t>Burger</t>
-  </si>
-  <si>
-    <t>Cheeseburger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pommes frites</t>
-  </si>
-  <si>
-    <t>19.-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street Food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baguette merguez</t>
-  </si>
-  <si>
-    <t>13.-</t>
-  </si>
-  <si>
-    <t>Mardi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bo Bun au boeuf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saladine de roquette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panini mozzarella et pesto rosso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salade mêlée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chicken Lousiana burger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shrimps Po' Boy</t>
-  </si>
-  <si>
-    <t>Mercredi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Couscous à l'agneau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tajine de légumes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schnitzel de poulet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pommes duchesse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hot fondue</t>
-  </si>
-  <si>
-    <t>Jeudi</t>
-  </si>
-  <si>
-    <t>Gyros</t>
-  </si>
-  <si>
     <t xml:space="preserve">BBQ pulled pork burger</t>
   </si>
   <si>
@@ -152,20 +154,18 @@
   </si>
   <si>
     <t xml:space="preserve">Saladine croquante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curry de poulet panang </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="8">
     <font>
-      <sz val="12.000000"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -177,6 +177,11 @@
       <b/>
       <sz val="12.000000"/>
       <color indexed="5"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12.000000"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
@@ -230,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -242,6 +247,19 @@
       <left style="thick">
         <color auto="1"/>
       </left>
+      <right style="none"/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right style="hair">
         <color auto="1"/>
       </right>
@@ -282,13 +300,15 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left style="hair">
+      <left style="thick">
         <color auto="1"/>
       </left>
-      <right style="hair">
+      <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="none"/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
       <bottom style="hair">
         <color auto="1"/>
       </bottom>
@@ -298,19 +318,6 @@
       <left style="thick">
         <color auto="1"/>
       </left>
-      <right style="none"/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
       <right style="hair">
         <color auto="1"/>
       </right>
@@ -335,90 +342,52 @@
       <bottom style="hair">
         <color auto="1"/>
       </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="none"/>
       <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
-    </xf>
-    <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf fontId="1" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="4" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="7" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="3" fillId="4" borderId="7" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="7" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="3" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="4" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="5" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="6" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="7" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,49 +691,49 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="">
+    <a:clrScheme name="New Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface="Arial"/>
         <a:cs typeface="Arial"/>
       </a:majorFont>
@@ -774,7 +743,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -783,67 +752,76 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:ln w="25400">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -880,11 +858,38 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:solidFill>
-          <a:srgbClr val="000000"/>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -895,409 +900,399 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A1" zoomScale="164" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="21.33203125"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="24.5"/>
-    <col customWidth="1" min="3" max="4" style="2" width="40.83203125"/>
-    <col customWidth="1" min="5" max="5" style="1" width="12.5"/>
-    <col customWidth="1" min="6" max="6" style="1" width="19.1640625"/>
-    <col min="7" max="16384" style="1" width="10.5"/>
+    <col customWidth="1" min="3" max="3" width="27.421875"/>
+    <col customWidth="1" min="4" max="4" width="27.28125"/>
+    <col customWidth="1" min="6" max="6" width="27.57421875"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="17">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" ht="15">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" ht="15">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" ht="15">
+      <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" s="8" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" ht="15">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="17" t="s">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" ht="15">
+      <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" ht="30">
+      <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="17" t="s">
+    <row r="8" ht="30">
+      <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="17" t="s">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" ht="15">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" ht="15">
+      <c r="A10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" ht="15">
+      <c r="A11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="18" t="s">
+    <row r="12" ht="15">
+      <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="18" t="s">
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" ht="15">
+      <c r="A13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="20" t="s">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" ht="15">
+      <c r="A14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="20" t="s">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" ht="30">
+      <c r="A15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14" t="s">
+      <c r="C15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="20" t="s">
+    <row r="16" ht="15">
+      <c r="A16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="20" t="s">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" ht="15">
+      <c r="A17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14" t="s">
+      <c r="C17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" ht="15">
+      <c r="A18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" ht="15">
+      <c r="A19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="14" t="s">
+      <c r="C19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="10" t="s">
+    <row r="20" ht="15">
+      <c r="A20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" s="19" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" ht="15">
+      <c r="A21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="D21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="30" ht="15">
-      <c r="C30" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="F21" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{002F00FC-00C2-49E5-809B-0029004B00AC}">
+          <x14:cfRule type="expression" priority="6" id="{009C001B-00EC-4CD4-85D5-0000001D00E0}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1308,7 +1303,7 @@
           <xm:sqref>E2:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{009D0034-0038-4E05-8A9A-007000270011}">
+          <x14:cfRule type="expression" priority="6" id="{00FD0043-007E-40F4-8DB1-000E00FF0019}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1319,7 +1314,7 @@
           <xm:sqref>F6 F8:F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{000D007E-0050-4ABC-AB5A-00E600240073}">
+          <x14:cfRule type="expression" priority="6" id="{00110013-007A-4CDB-AE15-00D3002B0036}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1330,7 +1325,7 @@
           <xm:sqref>F10 F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{004C00AD-00F6-489F-A7F7-002F00DF007E}">
+          <x14:cfRule type="expression" priority="6" id="{00FA0094-003B-461A-81E2-00DA00F00039}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1341,7 +1336,7 @@
           <xm:sqref>F14 F16:F17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{00A90056-004B-4C98-BD2D-004F00D60041}">
+          <x14:cfRule type="expression" priority="6" id="{009A00C8-00F7-4380-A9CA-00DB00940058}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1352,7 +1347,7 @@
           <xm:sqref>F18 F20:F21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{00720015-0095-48FE-82E4-006000C60072}">
+          <x14:cfRule type="expression" priority="6" id="{008B00E7-00C4-4154-8E69-008100D600F6}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1363,7 +1358,7 @@
           <xm:sqref>E6:E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{00C90083-0061-474B-B2DC-00E300FB00B9}">
+          <x14:cfRule type="expression" priority="6" id="{006E00DC-000D-4F35-B988-00FA00BB00F0}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1374,7 +1369,7 @@
           <xm:sqref>E10:E13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{00EA002C-008D-45A8-9608-00E000B20040}">
+          <x14:cfRule type="expression" priority="6" id="{00490013-00C4-4AF1-A061-003000B600FE}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1385,7 +1380,7 @@
           <xm:sqref>E14:E17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{003900A6-0067-4DC6-A158-0011007B0064}">
+          <x14:cfRule type="expression" priority="6" id="{00DB0073-003E-4CE5-A814-007600EE0058}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1396,7 +1391,7 @@
           <xm:sqref>E18:E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{0055009E-00C5-409B-B9DA-00B00006002E}">
+          <x14:cfRule type="expression" priority="6" id="{00A800F4-00AD-40B8-8324-00C500F40015}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1407,7 +1402,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{002400D4-004E-47E3-97F4-00CB008200C0}">
+          <x14:cfRule type="expression" priority="6" id="{00FA000B-004F-4DFC-9934-007300EF0068}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1418,7 +1413,7 @@
           <xm:sqref>F11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{00A60093-0030-4242-8A61-000400B40000}">
+          <x14:cfRule type="expression" priority="6" id="{00580040-0026-4500-9190-0013003B0005}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1429,7 +1424,7 @@
           <xm:sqref>F15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{003900AA-0048-440B-B394-00A200A400AB}">
+          <x14:cfRule type="expression" priority="6" id="{000900D5-00A4-4EF4-9413-003100B60014}">
             <xm:f>E2=0</xm:f>
             <x14:dxf>
               <font>
@@ -1440,7 +1435,7 @@
           <xm:sqref>F19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00E1003F-0004-4320-9513-0066005B004F}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00B000F9-0067-4048-87B1-0073009B0098}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1457,7 +1452,7 @@
           <xm:sqref>E2:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{0059008E-00C1-4658-93F2-00EC000A0086}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00C2004D-0058-49BC-AB09-004D006D0056}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1474,7 +1469,7 @@
           <xm:sqref>F6 F8:F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{006D005D-0095-49C2-B7E6-000200920075}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{009B00EC-00F8-4686-BBE1-00B800600093}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1491,7 +1486,7 @@
           <xm:sqref>F10 F12:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{0097007E-0089-4F48-9DB2-00DE00000039}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{005A00AC-006A-49C2-AB92-0095001D00AE}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1508,7 +1503,7 @@
           <xm:sqref>F14 F16:F17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{006F00E5-00C1-4FE8-813A-008200E400E4}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00DD00FD-00A5-4687-A1A4-00AB001F0005}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1525,7 +1520,7 @@
           <xm:sqref>F18 F20:F21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{0008007D-0067-4F93-85F8-00D900D200CC}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00360090-007E-43A2-A561-0030004A0012}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1542,7 +1537,7 @@
           <xm:sqref>E6:E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{004D0028-001D-4314-8A56-00C0007F00F9}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00F00000-00B5-4B41-9FB7-00C9004900DE}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1559,7 +1554,7 @@
           <xm:sqref>E10:E13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{007300FD-0010-4E8F-B272-00920006001D}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{000500EF-003F-44FF-83C3-0093009500D3}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1576,7 +1571,7 @@
           <xm:sqref>E14:E17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{000D004B-005D-4D41-9461-0078007F00F4}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{005200C3-0050-4F40-9D3F-0052009B005F}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1593,7 +1588,7 @@
           <xm:sqref>E18:E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{008400CB-00AF-408B-8FD4-00310024002F}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00500073-00B1-4B72-B712-002000F4009A}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1610,7 +1605,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00C60090-0067-4BA8-BF3C-003F008B002E}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00C5002B-00B5-4BF2-AB2F-00B5003C00FA}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1627,7 +1622,7 @@
           <xm:sqref>F11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{00260071-0029-4132-8834-002C0022006E}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{005D004F-0049-4AFE-ADE3-005A00BE004A}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>
@@ -1644,7 +1639,7 @@
           <xm:sqref>F15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{007600F7-004E-4446-B2C5-000300E900A9}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" text="," id="{008C0076-0006-45F1-A441-004300A100E4}">
             <xm:f>NOT(ISERROR(SEARCH(",",E2)))</xm:f>
             <x14:dxf>
               <font>

</xml_diff>